<commit_message>
limpieza de datos y creación de main.py
</commit_message>
<xml_diff>
--- a/dataweb.xlsx
+++ b/dataweb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H254"/>
+  <dimension ref="A1:H253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8 may 2025</t>
+          <t>9 may 2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>60,28</t>
+          <t>60,33</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,17 +496,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>60,15</t>
+          <t>60,32</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>60,15</t>
+          <t>60,32</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>10.088</t>
+          <t>13.425</t>
         </is>
       </c>
     </row>
@@ -10547,46 +10547,6 @@
       <c r="H253" t="inlineStr">
         <is>
           <t>272.712</t>
-        </is>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" s="1" t="n">
-        <v>252</v>
-      </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>8 may 2024</t>
-        </is>
-      </c>
-      <c r="C254" t="inlineStr">
-        <is>
-          <t>78,34</t>
-        </is>
-      </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>79,27</t>
-        </is>
-      </c>
-      <c r="E254" t="inlineStr">
-        <is>
-          <t>76,89</t>
-        </is>
-      </c>
-      <c r="F254" t="inlineStr">
-        <is>
-          <t>78,99</t>
-        </is>
-      </c>
-      <c r="G254" t="inlineStr">
-        <is>
-          <t>78,99</t>
-        </is>
-      </c>
-      <c r="H254" t="inlineStr">
-        <is>
-          <t>355.449</t>
         </is>
       </c>
     </row>

</xml_diff>